<commit_message>
Fixed issue with end of block
</commit_message>
<xml_diff>
--- a/Subjects/subject 1/processed_audio_df.xlsx
+++ b/Subjects/subject 1/processed_audio_df.xlsx
@@ -482,7 +482,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -554,7 +554,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -590,7 +590,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -626,7 +626,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J7" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
@@ -662,7 +662,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J8" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -698,7 +698,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
@@ -734,7 +734,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11">
@@ -770,7 +770,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -806,7 +806,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J12" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -842,7 +842,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J13" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
@@ -878,7 +878,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -914,7 +914,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J15" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -986,7 +986,7 @@
         <v>1.72</v>
       </c>
       <c r="J17" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1022,7 +1022,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J18" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1058,7 +1058,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J19" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -1094,7 +1094,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J20" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -1130,7 +1130,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J21" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -1166,7 +1166,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J22" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1202,7 +1202,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J23" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -1274,7 +1274,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1310,7 +1310,7 @@
         <v>1.72</v>
       </c>
       <c r="J26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1346,7 +1346,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J27" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -1382,7 +1382,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1526,7 +1526,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J32" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
@@ -1562,7 +1562,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J33" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34">
@@ -1598,7 +1598,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J34" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
@@ -1634,7 +1634,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J35" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
@@ -1670,7 +1670,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -1706,7 +1706,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J37" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
@@ -1742,7 +1742,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J38" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
@@ -1778,7 +1778,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J39" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1814,7 +1814,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J40" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
@@ -1886,7 +1886,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J42" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43">
@@ -1922,7 +1922,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J43" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
@@ -1958,7 +1958,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
@@ -1994,7 +1994,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J45" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -2030,7 +2030,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J46" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -2066,7 +2066,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J47" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48">
@@ -2102,7 +2102,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J48" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49">
@@ -2138,7 +2138,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J49" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -2174,7 +2174,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J50" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -2210,7 +2210,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J51" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52">
@@ -2282,7 +2282,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J53" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
@@ -2318,7 +2318,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J54" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55">
@@ -2354,7 +2354,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
@@ -2390,7 +2390,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J56" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
@@ -2462,7 +2462,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J58" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -2498,7 +2498,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J59" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60">
@@ -2534,7 +2534,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J60" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61">
@@ -2570,7 +2570,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J61" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
@@ -2606,7 +2606,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J62" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63">
@@ -2642,7 +2642,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J63" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
@@ -2678,7 +2678,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J64" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65">
@@ -2750,7 +2750,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J66" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67">
@@ -2786,7 +2786,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J67" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="68">
@@ -2822,7 +2822,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J68" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69">
@@ -2858,7 +2858,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J69" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70">
@@ -2894,7 +2894,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J70" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
@@ -2930,7 +2930,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J71" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -2966,7 +2966,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J72" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -3002,7 +3002,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J73" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3074,7 +3074,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J75" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
@@ -3110,7 +3110,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J76" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
@@ -3146,7 +3146,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J77" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
@@ -3218,7 +3218,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J79" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80">
@@ -3254,7 +3254,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J80" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81">

</xml_diff>

<commit_message>
Upadting keys and space binds, full screen and cursor disable
</commit_message>
<xml_diff>
--- a/Subjects/subject 1/processed_audio_df.xlsx
+++ b/Subjects/subject 1/processed_audio_df.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -446,7 +446,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J2" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -482,7 +482,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -518,7 +518,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +554,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J5" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -590,7 +590,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J6" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -626,7 +626,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -662,7 +662,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -698,7 +698,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -770,7 +770,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J11" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -806,7 +806,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J12" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -842,7 +842,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J13" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -878,7 +878,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -914,7 +914,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -950,7 +950,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -986,7 +986,7 @@
         <v>1.72</v>
       </c>
       <c r="J17" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1022,7 +1022,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J18" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -1058,7 +1058,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J19" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
@@ -1094,7 +1094,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -1166,7 +1166,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J22" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -1238,7 +1238,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J24" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -1274,7 +1274,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J25" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -1310,7 +1310,7 @@
         <v>1.72</v>
       </c>
       <c r="J26" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
@@ -1346,7 +1346,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J27" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28">
@@ -1382,7 +1382,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J28" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
@@ -1418,7 +1418,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J29" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
@@ -1454,7 +1454,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J30" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
@@ -1490,7 +1490,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -1526,7 +1526,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J32" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
@@ -1562,7 +1562,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J33" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1634,7 +1634,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J35" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1670,7 +1670,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37">
@@ -1706,7 +1706,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J37" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
@@ -1742,7 +1742,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J38" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
@@ -1778,7 +1778,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J39" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -1814,7 +1814,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J40" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
@@ -1850,7 +1850,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J41" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -1886,7 +1886,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J42" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -1922,7 +1922,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J43" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -1958,7 +1958,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J44" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
@@ -1994,7 +1994,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J45" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
@@ -2030,7 +2030,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J46" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
@@ -2066,7 +2066,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J47" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
@@ -2102,7 +2102,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J48" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49">
@@ -2138,7 +2138,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -2174,7 +2174,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J50" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
@@ -2210,7 +2210,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J51" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52">
@@ -2246,7 +2246,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J52" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -2282,7 +2282,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J53" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -2354,7 +2354,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J55" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56">
@@ -2390,7 +2390,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J56" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -2426,7 +2426,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
@@ -2462,7 +2462,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J58" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -2498,7 +2498,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J59" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60">
@@ -2534,7 +2534,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J60" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61">
@@ -2570,7 +2570,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J61" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -2606,7 +2606,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J62" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63">
@@ -2642,7 +2642,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J63" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
@@ -2678,7 +2678,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J64" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65">
@@ -2750,7 +2750,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J66" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67">
@@ -2786,7 +2786,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J67" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68">
@@ -2822,7 +2822,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J68" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69">
@@ -2858,7 +2858,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J69" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -2894,7 +2894,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J70" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71">
@@ -2930,7 +2930,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J71" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -2966,7 +2966,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J72" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73">
@@ -3002,7 +3002,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J73" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3038,7 +3038,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J74" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75">
@@ -3074,7 +3074,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J75" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76">
@@ -3110,7 +3110,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J76" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77">
@@ -3146,7 +3146,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J77" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78">
@@ -3182,7 +3182,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J78" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79">
@@ -3218,7 +3218,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J79" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80">
@@ -3254,7 +3254,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J80" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -3294,6 +3294,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update allocation, instruction image (spacebar)
</commit_message>
<xml_diff>
--- a/Subjects/subject 1/processed_audio_df.xlsx
+++ b/Subjects/subject 1/processed_audio_df.xlsx
@@ -446,7 +446,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J2" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -482,7 +482,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -518,7 +518,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +554,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J5" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -698,7 +698,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J9" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -734,7 +734,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -806,7 +806,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J12" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13">
@@ -842,7 +842,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
@@ -878,7 +878,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
@@ -914,7 +914,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J15" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -950,7 +950,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J16" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -986,7 +986,7 @@
         <v>1.72</v>
       </c>
       <c r="J17" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
@@ -1058,7 +1058,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J19" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
@@ -1094,7 +1094,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J20" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -1130,7 +1130,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J21" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
@@ -1166,7 +1166,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J22" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1202,7 +1202,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J23" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
@@ -1238,7 +1238,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J24" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
@@ -1274,7 +1274,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
@@ -1346,7 +1346,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -1382,7 +1382,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J28" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29">
@@ -1418,7 +1418,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J29" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
@@ -1454,7 +1454,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31">
@@ -1490,7 +1490,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J31" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
@@ -1526,7 +1526,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J32" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
@@ -1562,7 +1562,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J33" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34">
@@ -1598,7 +1598,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J34" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -1634,7 +1634,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J35" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36">
@@ -1670,7 +1670,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
@@ -1706,7 +1706,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J37" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -1742,7 +1742,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J38" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1778,7 +1778,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -1850,7 +1850,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J41" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -1922,7 +1922,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J43" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
@@ -1994,7 +1994,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J45" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46">
@@ -2030,7 +2030,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47">
@@ -2066,7 +2066,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
@@ -2102,7 +2102,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J48" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -2138,7 +2138,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J49" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -2246,7 +2246,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J52" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
@@ -2282,7 +2282,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J53" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54">
@@ -2354,7 +2354,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J55" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
@@ -2462,7 +2462,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J58" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
@@ -2498,7 +2498,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J59" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60">
@@ -2534,7 +2534,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J60" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61">
@@ -2570,7 +2570,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J61" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62">
@@ -2606,7 +2606,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J62" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63">
@@ -2642,7 +2642,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -2678,7 +2678,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J64" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="65">
@@ -2714,7 +2714,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J65" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
@@ -2750,7 +2750,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J66" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
@@ -2786,7 +2786,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J67" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68">
@@ -2822,7 +2822,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J68" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69">
@@ -2858,7 +2858,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J69" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
@@ -2894,7 +2894,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J70" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="71">
@@ -2930,7 +2930,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J71" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72">
@@ -2966,7 +2966,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J72" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
@@ -3002,7 +3002,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J73" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74">
@@ -3110,7 +3110,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J76" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77">
@@ -3146,7 +3146,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J77" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78">
@@ -3182,7 +3182,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J78" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79">
@@ -3218,7 +3218,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J79" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
@@ -3254,7 +3254,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J80" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
@@ -3290,7 +3290,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J81" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AFACT feddback timing updata and implementing in console
</commit_message>
<xml_diff>
--- a/Subjects/subject 1/processed_audio_df.xlsx
+++ b/Subjects/subject 1/processed_audio_df.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -54,18 +54,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -446,7 +446,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -482,7 +482,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -554,7 +554,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J5" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6">
@@ -590,7 +590,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -626,7 +626,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J7" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -662,7 +662,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -698,7 +698,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J9" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -734,7 +734,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -770,7 +770,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J11" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -806,7 +806,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J12" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -842,7 +842,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -878,7 +878,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -914,7 +914,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -950,7 +950,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J16" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -986,7 +986,7 @@
         <v>1.72</v>
       </c>
       <c r="J17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -1022,7 +1022,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J18" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -1058,7 +1058,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J19" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -1094,7 +1094,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -1166,7 +1166,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J22" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -1238,7 +1238,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J24" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1274,7 +1274,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J25" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
@@ -1418,7 +1418,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J29" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
@@ -1454,7 +1454,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J30" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
@@ -1490,7 +1490,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J31" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -1562,7 +1562,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J33" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
@@ -1634,7 +1634,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J35" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36">
@@ -1706,7 +1706,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J37" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
@@ -1742,7 +1742,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J38" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
@@ -1778,7 +1778,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
@@ -1814,7 +1814,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J40" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41">
@@ -1850,7 +1850,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J41" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42">
@@ -1886,7 +1886,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J42" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -1922,7 +1922,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J43" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44">
@@ -1958,7 +1958,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J44" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
@@ -1994,7 +1994,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J45" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46">
@@ -2030,7 +2030,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J46" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
@@ -2066,7 +2066,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J47" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -2138,7 +2138,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J49" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50">
@@ -2174,7 +2174,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J50" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
@@ -2246,7 +2246,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J52" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53">
@@ -2282,7 +2282,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J53" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
@@ -2318,7 +2318,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J54" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
@@ -2354,7 +2354,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J55" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
@@ -2426,7 +2426,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J57" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58">
@@ -2462,7 +2462,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J58" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
@@ -2498,7 +2498,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J59" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60">
@@ -2534,7 +2534,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J60" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
@@ -2570,7 +2570,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J61" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62">
@@ -2606,7 +2606,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
@@ -2678,7 +2678,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J64" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65">
@@ -2714,7 +2714,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J65" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66">
@@ -2750,7 +2750,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J66" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67">
@@ -2786,7 +2786,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J67" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -2822,7 +2822,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J68" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69">
@@ -2858,7 +2858,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J69" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70">
@@ -2894,7 +2894,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J70" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -2930,7 +2930,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J71" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
@@ -2966,7 +2966,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J72" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73">
@@ -3038,7 +3038,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J74" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75">
@@ -3074,7 +3074,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J75" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76">
@@ -3110,7 +3110,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J76" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77">
@@ -3146,7 +3146,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J77" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -3182,7 +3182,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J78" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79">
@@ -3218,7 +3218,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J79" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="80">
@@ -3254,7 +3254,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J80" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -3290,10 +3290,10 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J81" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
afact orgona; feedback stimuli
</commit_message>
<xml_diff>
--- a/Subjects/subject 1/processed_audio_df.xlsx
+++ b/Subjects/subject 1/processed_audio_df.xlsx
@@ -446,7 +446,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -482,7 +482,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J3" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -518,7 +518,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J4" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +554,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J5" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -590,7 +590,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
@@ -626,7 +626,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -662,7 +662,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -734,7 +734,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J10" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -770,7 +770,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J11" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -878,7 +878,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -914,7 +914,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J15" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
@@ -950,7 +950,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J16" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -986,7 +986,7 @@
         <v>1.72</v>
       </c>
       <c r="J17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1022,7 +1022,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J18" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -1058,7 +1058,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J19" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
@@ -1094,7 +1094,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
@@ -1166,7 +1166,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J22" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
@@ -1202,7 +1202,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J23" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -1238,7 +1238,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J24" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
@@ -1274,7 +1274,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J25" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -1310,7 +1310,7 @@
         <v>1.72</v>
       </c>
       <c r="J26" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1346,7 +1346,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
@@ -1382,7 +1382,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29">
@@ -1418,7 +1418,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J29" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
@@ -1454,7 +1454,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J30" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -1490,7 +1490,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J31" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32">
@@ -1526,7 +1526,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J32" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33">
@@ -1562,7 +1562,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J33" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -1598,7 +1598,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J34" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
@@ -1634,7 +1634,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J35" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -1670,7 +1670,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J36" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
@@ -1706,7 +1706,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J37" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -1742,7 +1742,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J38" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39">
@@ -1778,7 +1778,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40">
@@ -1814,7 +1814,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J40" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41">
@@ -1850,7 +1850,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J41" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -1886,7 +1886,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J42" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43">
@@ -1922,7 +1922,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J43" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
@@ -1958,7 +1958,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
@@ -1994,7 +1994,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J45" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46">
@@ -2030,7 +2030,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J46" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47">
@@ -2066,7 +2066,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J47" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
@@ -2102,7 +2102,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J48" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
@@ -2138,7 +2138,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J49" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
@@ -2174,7 +2174,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J50" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
@@ -2246,7 +2246,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J52" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53">
@@ -2282,7 +2282,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J53" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -2318,7 +2318,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J54" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55">
@@ -2354,7 +2354,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J55" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56">
@@ -2390,7 +2390,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J56" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57">
@@ -2426,7 +2426,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J57" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58">
@@ -2462,7 +2462,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
@@ -2498,7 +2498,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J59" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -2534,7 +2534,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J60" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2570,7 +2570,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J61" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -2606,7 +2606,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J62" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="63">
@@ -2678,7 +2678,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J64" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -2714,7 +2714,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J65" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -2750,7 +2750,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J66" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
@@ -2786,7 +2786,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J67" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
@@ -2822,7 +2822,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J68" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="69">
@@ -2858,7 +2858,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J69" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -2894,7 +2894,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J70" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
@@ -2930,7 +2930,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J71" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72">
@@ -2966,7 +2966,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J72" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73">
@@ -3002,7 +3002,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J73" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74">
@@ -3074,7 +3074,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J75" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76">
@@ -3146,7 +3146,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J77" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
@@ -3182,7 +3182,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J78" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
@@ -3218,7 +3218,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J79" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="80">
@@ -3254,7 +3254,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J80" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">

</xml_diff>

<commit_message>
Afact original gui updated
</commit_message>
<xml_diff>
--- a/Subjects/subject 1/processed_audio_df.xlsx
+++ b/Subjects/subject 1/processed_audio_df.xlsx
@@ -446,7 +446,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J2" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -482,7 +482,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J3" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -518,7 +518,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -590,7 +590,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
@@ -626,7 +626,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J7" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -662,7 +662,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -698,7 +698,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -734,7 +734,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -770,7 +770,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -806,7 +806,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J12" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -842,7 +842,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J13" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
@@ -878,7 +878,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -914,7 +914,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J15" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -950,7 +950,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J16" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
@@ -986,7 +986,7 @@
         <v>1.72</v>
       </c>
       <c r="J17" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -1022,7 +1022,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J18" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -1058,7 +1058,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J19" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
@@ -1094,7 +1094,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J20" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
@@ -1166,7 +1166,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J22" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
@@ -1202,7 +1202,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J23" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -1238,7 +1238,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J24" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
@@ -1310,7 +1310,7 @@
         <v>1.72</v>
       </c>
       <c r="J26" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -1382,7 +1382,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J28" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29">
@@ -1418,7 +1418,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J29" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30">
@@ -1454,7 +1454,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J30" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31">
@@ -1526,7 +1526,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J32" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
@@ -1562,7 +1562,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J33" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34">
@@ -1598,7 +1598,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J34" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
@@ -1634,7 +1634,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J35" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -1670,7 +1670,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J36" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -1706,7 +1706,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J37" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
@@ -1742,7 +1742,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J38" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -1778,7 +1778,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J39" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -1814,7 +1814,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J40" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
@@ -1886,7 +1886,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J42" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">
@@ -1922,7 +1922,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J43" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -1958,7 +1958,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J44" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
@@ -1994,7 +1994,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J45" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
@@ -2030,7 +2030,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J46" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47">
@@ -2066,7 +2066,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J47" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
@@ -2102,7 +2102,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J48" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49">
@@ -2174,7 +2174,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J50" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -2282,7 +2282,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J53" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54">
@@ -2318,7 +2318,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J54" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55">
@@ -2426,7 +2426,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J57" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58">
@@ -2462,7 +2462,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J58" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59">
@@ -2498,7 +2498,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J59" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60">
@@ -2534,7 +2534,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J60" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61">
@@ -2570,7 +2570,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J61" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
@@ -2606,7 +2606,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J62" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63">
@@ -2678,7 +2678,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J64" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65">
@@ -2714,7 +2714,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J65" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
@@ -2822,7 +2822,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J68" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
@@ -2858,7 +2858,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J69" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70">
@@ -2894,7 +2894,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J70" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71">
@@ -2930,7 +2930,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J71" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72">
@@ -2966,7 +2966,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J72" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
@@ -3038,7 +3038,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J74" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
@@ -3074,7 +3074,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J75" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76">
@@ -3110,7 +3110,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J76" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -3146,7 +3146,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J77" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78">
@@ -3218,7 +3218,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J79" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80">
@@ -3254,7 +3254,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J80" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81">
@@ -3290,7 +3290,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J81" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
omer processed audio df
</commit_message>
<xml_diff>
--- a/Subjects/subject 1/processed_audio_df.xlsx
+++ b/Subjects/subject 1/processed_audio_df.xlsx
@@ -446,7 +446,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -482,7 +482,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J3" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
@@ -518,7 +518,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -554,7 +554,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J5" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -590,7 +590,7 @@
         <v>2.75734693877551</v>
       </c>
       <c r="J6" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
@@ -626,7 +626,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J7" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -734,7 +734,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
@@ -770,7 +770,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -842,7 +842,7 @@
         <v>2.752018140589569</v>
       </c>
       <c r="J13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -878,7 +878,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J14" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -914,7 +914,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J15" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16">
@@ -950,7 +950,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J16" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
@@ -986,7 +986,7 @@
         <v>1.72</v>
       </c>
       <c r="J17" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18">
@@ -1022,7 +1022,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
@@ -1058,7 +1058,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J19" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -1094,7 +1094,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J20" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
@@ -1130,7 +1130,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J21" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
@@ -1166,7 +1166,7 @@
         <v>1.906666666666667</v>
       </c>
       <c r="J22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23">
@@ -1202,7 +1202,7 @@
         <v>1.738684807256236</v>
       </c>
       <c r="J23" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -1238,7 +1238,7 @@
         <v>1.904013605442177</v>
       </c>
       <c r="J24" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
@@ -1274,7 +1274,7 @@
         <v>2.914671201814059</v>
       </c>
       <c r="J25" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
@@ -1310,7 +1310,7 @@
         <v>1.72</v>
       </c>
       <c r="J26" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
@@ -1346,7 +1346,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
@@ -1382,7 +1382,7 @@
         <v>2.24265306122449</v>
       </c>
       <c r="J28" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
@@ -1418,7 +1418,7 @@
         <v>1.733333333333333</v>
       </c>
       <c r="J29" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
@@ -1490,7 +1490,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J31" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
@@ -1562,7 +1562,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J33" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
@@ -1598,7 +1598,7 @@
         <v>2.234671201814059</v>
       </c>
       <c r="J34" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
@@ -1634,7 +1634,7 @@
         <v>2.07734693877551</v>
       </c>
       <c r="J35" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
@@ -1670,7 +1670,7 @@
         <v>1.72265306122449</v>
       </c>
       <c r="J36" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
@@ -1742,7 +1742,7 @@
         <v>1.552018140589569</v>
       </c>
       <c r="J38" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -1778,7 +1778,7 @@
         <v>2.066666666666667</v>
       </c>
       <c r="J39" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -1814,7 +1814,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J40" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
@@ -1850,7 +1850,7 @@
         <v>1.901337868480726</v>
       </c>
       <c r="J41" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
@@ -1886,7 +1886,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J42" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43">
@@ -1922,7 +1922,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J43" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44">
@@ -1958,7 +1958,7 @@
         <v>1.893333333333334</v>
       </c>
       <c r="J44" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -1994,7 +1994,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J45" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46">
@@ -2066,7 +2066,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J47" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
@@ -2102,7 +2102,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J48" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49">
@@ -2138,7 +2138,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J49" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50">
@@ -2174,7 +2174,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J50" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
@@ -2210,7 +2210,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J51" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
@@ -2246,7 +2246,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J52" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
@@ -2282,7 +2282,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J53" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
@@ -2354,7 +2354,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J55" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
@@ -2390,7 +2390,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J56" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
@@ -2426,7 +2426,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J57" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58">
@@ -2462,7 +2462,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J58" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59">
@@ -2498,7 +2498,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J59" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="60">
@@ -2534,7 +2534,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J60" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -2570,7 +2570,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J61" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -2606,7 +2606,7 @@
         <v>1.565351473922902</v>
       </c>
       <c r="J62" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63">
@@ -2642,7 +2642,7 @@
         <v>1.890680272108844</v>
       </c>
       <c r="J63" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64">
@@ -2678,7 +2678,7 @@
         <v>1.549319727891156</v>
       </c>
       <c r="J64" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -2714,7 +2714,7 @@
         <v>1.218684807256236</v>
       </c>
       <c r="J65" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -2750,7 +2750,7 @@
         <v>1.735986394557823</v>
       </c>
       <c r="J66" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67">
@@ -2786,7 +2786,7 @@
         <v>1.730680272108843</v>
       </c>
       <c r="J67" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68">
@@ -2822,7 +2822,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J68" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -2858,7 +2858,7 @@
         <v>1.56265306122449</v>
       </c>
       <c r="J69" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="70">
@@ -2894,7 +2894,7 @@
         <v>1.226666666666667</v>
       </c>
       <c r="J70" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71">
@@ -2930,7 +2930,7 @@
         <v>1.213333333333333</v>
       </c>
       <c r="J71" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="72">
@@ -2966,7 +2966,7 @@
         <v>1.055986394557823</v>
       </c>
       <c r="J72" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73">
@@ -3002,7 +3002,7 @@
         <v>2.069319727891156</v>
       </c>
       <c r="J73" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -3038,7 +3038,7 @@
         <v>1.728004535147392</v>
       </c>
       <c r="J74" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
@@ -3074,7 +3074,7 @@
         <v>1.389319727891156</v>
       </c>
       <c r="J75" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="76">
@@ -3110,7 +3110,7 @@
         <v>1.208004535147392</v>
       </c>
       <c r="J76" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
@@ -3146,7 +3146,7 @@
         <v>1.386666666666667</v>
       </c>
       <c r="J77" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
@@ -3182,7 +3182,7 @@
         <v>1.215986394557823</v>
       </c>
       <c r="J78" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79">
@@ -3254,7 +3254,7 @@
         <v>1.725351473922903</v>
       </c>
       <c r="J80" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
@@ -3290,7 +3290,7 @@
         <v>3.272018140589569</v>
       </c>
       <c r="J81" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>